<commit_message>
completed dashboard all 3 scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/controller.xlsx
+++ b/src/test/resources/testdata/controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prdp4\IdeaProjects\CucumberMiniProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3C82C7-05B7-4C22-9A99-35E5DC617A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE8AFA-DC53-4C5F-A07C-AC895D1F3735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>item-name</t>
   </si>
   <si>
-    <t>lenovo</t>
+    <t>Lenovo Thinkpad X1 Carbon Laptop</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:XFD1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
checkout one scenario completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/controller.xlsx
+++ b/src/test/resources/testdata/controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prdp4\IdeaProjects\CucumberMiniProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE8AFA-DC53-4C5F-A07C-AC895D1F3735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40850718-CA5A-416B-A503-2F17AE248DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>userAccount</t>
   </si>
@@ -43,6 +43,33 @@
   </si>
   <si>
     <t>Lenovo Thinkpad X1 Carbon Laptop</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>mob</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>560001</t>
+  </si>
+  <si>
+    <t>9999999999</t>
   </si>
 </sst>
 </file>
@@ -361,19 +388,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,8 +412,23 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -393,6 +437,21 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>